<commit_message>
Set default to weather scan to a single weather file...Added potential to store base64 data into CSV...commented it out becuase I think it may be a bad idea.
</commit_message>
<xml_diff>
--- a/projects/NECB_Full_WeatherFile_Scan.xlsx
+++ b/projects/NECB_Full_WeatherFile_Scan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="5430" windowWidth="20370" windowHeight="5085" tabRatio="469" activeTab="5"/>
+    <workbookView xWindow="-15" yWindow="5430" windowWidth="20370" windowHeight="5085" tabRatio="469" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="9" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1093" uniqueCount="556">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1098" uniqueCount="557">
   <si>
     <t>type</t>
   </si>
@@ -1705,6 +1705,9 @@
   </si>
   <si>
     <t>Building Types</t>
+  </si>
+  <si>
+    <t>btapresults.zipped_model_osm</t>
   </si>
 </sst>
 </file>
@@ -4302,10 +4305,10 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="31" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="27" fillId="45" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="46" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="46" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1842">
     <cellStyle name="20% - Accent1" xfId="1819" builtinId="30" customBuiltin="1"/>
@@ -7014,8 +7017,8 @@
   </sheetPr>
   <dimension ref="A1:Z10"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScaleNormal="100" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -7070,14 +7073,14 @@
       <c r="R1" s="5"/>
       <c r="S1" s="5"/>
       <c r="T1" s="5"/>
-      <c r="U1" s="67" t="s">
+      <c r="U1" s="68" t="s">
         <v>40</v>
       </c>
-      <c r="V1" s="67"/>
-      <c r="W1" s="67"/>
-      <c r="X1" s="67"/>
-      <c r="Y1" s="67"/>
-      <c r="Z1" s="67"/>
+      <c r="V1" s="68"/>
+      <c r="W1" s="68"/>
+      <c r="X1" s="68"/>
+      <c r="Y1" s="68"/>
+      <c r="Z1" s="68"/>
     </row>
     <row r="2" spans="1:26" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
@@ -7351,7 +7354,7 @@
     </row>
     <row r="9" spans="1:26" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="62" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B9" s="58" t="s">
         <v>418</v>
@@ -7370,7 +7373,7 @@
     </row>
     <row r="10" spans="1:26" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="62" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B10" s="49" t="s">
         <v>240</v>
@@ -7419,11 +7422,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M282"/>
+  <dimension ref="A1:M283"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A221" sqref="A221"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="120" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A238" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D283" sqref="A283:D283"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12977,6 +12980,32 @@
         <v>1</v>
       </c>
       <c r="I282" s="64" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="283" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A283" s="29" t="s">
+        <v>556</v>
+      </c>
+      <c r="B283" s="29" t="s">
+        <v>556</v>
+      </c>
+      <c r="C283" s="29" t="s">
+        <v>556</v>
+      </c>
+      <c r="D283" s="29" t="s">
+        <v>556</v>
+      </c>
+      <c r="F283" s="29" t="s">
+        <v>428</v>
+      </c>
+      <c r="G283" s="64" t="b">
+        <v>1</v>
+      </c>
+      <c r="H283" s="64" t="b">
+        <v>1</v>
+      </c>
+      <c r="I283" s="64" t="b">
         <v>0</v>
       </c>
     </row>
@@ -13496,7 +13525,7 @@
   </sheetPr>
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
@@ -13506,7 +13535,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="67" t="s">
         <v>526</v>
       </c>
       <c r="B1" t="s">
@@ -13514,7 +13543,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="68" t="s">
+      <c r="A2" s="67" t="s">
         <v>528</v>
       </c>
       <c r="B2" t="s">
@@ -13522,10 +13551,10 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="68"/>
+      <c r="A3" s="67"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="68" t="s">
+      <c r="A4" s="67" t="s">
         <v>529</v>
       </c>
       <c r="B4" t="s">
@@ -13533,7 +13562,7 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="68" t="s">
+      <c r="A5" s="67" t="s">
         <v>531</v>
       </c>
       <c r="B5" t="s">
@@ -13541,7 +13570,7 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="68" t="s">
+      <c r="A6" s="67" t="s">
         <v>533</v>
       </c>
       <c r="B6" t="s">
@@ -13549,7 +13578,7 @@
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="68" t="s">
+      <c r="A7" s="67" t="s">
         <v>535</v>
       </c>
       <c r="B7" t="s">
@@ -13557,7 +13586,7 @@
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="68" t="s">
+      <c r="A8" s="67" t="s">
         <v>537</v>
       </c>
       <c r="B8" t="s">
@@ -13565,7 +13594,7 @@
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="68" t="s">
+      <c r="A9" s="67" t="s">
         <v>539</v>
       </c>
       <c r="B9" t="s">
@@ -13573,7 +13602,7 @@
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="68" t="s">
+      <c r="A10" s="67" t="s">
         <v>541</v>
       </c>
       <c r="B10" t="s">
@@ -13581,7 +13610,7 @@
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="68" t="s">
+      <c r="A11" s="67" t="s">
         <v>543</v>
       </c>
       <c r="B11" t="s">
@@ -13589,7 +13618,7 @@
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="68" t="s">
+      <c r="A12" s="67" t="s">
         <v>545</v>
       </c>
       <c r="B12" t="s">
@@ -13597,7 +13626,7 @@
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="68" t="s">
+      <c r="A13" s="67" t="s">
         <v>547</v>
       </c>
       <c r="B13" t="s">
@@ -13605,7 +13634,7 @@
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="68" t="s">
+      <c r="A14" s="67" t="s">
         <v>549</v>
       </c>
       <c r="B14" t="s">
@@ -13613,7 +13642,7 @@
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="68" t="s">
+      <c r="A15" s="67" t="s">
         <v>551</v>
       </c>
       <c r="B15" t="s">
@@ -13621,7 +13650,7 @@
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="68" t="s">
+      <c r="A16" s="67" t="s">
         <v>553</v>
       </c>
       <c r="B16" t="s">
@@ -13629,13 +13658,13 @@
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="68"/>
+      <c r="A17" s="67"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="68"/>
+      <c r="A18" s="67"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="68" t="s">
+      <c r="A19" s="67" t="s">
         <v>555</v>
       </c>
       <c r="B19" t="s">

</xml_diff>

<commit_message>
Commented out Base64 implementation that works (sort of ) with CSV files. This would require a post process of the csv file before it is usable.
</commit_message>
<xml_diff>
--- a/projects/NECB_Full_WeatherFile_Scan.xlsx
+++ b/projects/NECB_Full_WeatherFile_Scan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="5430" windowWidth="20370" windowHeight="5085" tabRatio="469" activeTab="3"/>
+    <workbookView xWindow="-15" yWindow="5430" windowWidth="20370" windowHeight="5085" tabRatio="469" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="9" r:id="rId1"/>
@@ -1302,9 +1302,6 @@
     <t>Phylroy-NECB Analysis</t>
   </si>
   <si>
-    <t>Phylroys_Cluster</t>
-  </si>
-  <si>
     <t>plopez</t>
   </si>
   <si>
@@ -1708,6 +1705,9 @@
   </si>
   <si>
     <t>btapresults.zipped_model_osm</t>
+  </si>
+  <si>
+    <t>phylroys_mini_cluster</t>
   </si>
 </sst>
 </file>
@@ -6555,8 +6555,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6603,7 +6603,7 @@
         <v>66</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>67</v>
@@ -6625,7 +6625,7 @@
         <v>78</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>421</v>
+        <v>556</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>80</v>
@@ -6809,7 +6809,7 @@
         <v>62</v>
       </c>
       <c r="C23" s="44" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="D23" s="31" t="s">
         <v>62</v>
@@ -7346,7 +7346,7 @@
         <v>1</v>
       </c>
       <c r="P8" s="51" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="R8" s="50" t="s">
         <v>214</v>
@@ -7424,7 +7424,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M283"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="120" workbookViewId="0">
+    <sheetView zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="120" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A238" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D283" sqref="A283:D283"/>
     </sheetView>
@@ -11027,14 +11027,14 @@
     </row>
     <row r="198" spans="1:13" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A198" s="60" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B198" s="60" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C198" s="60"/>
       <c r="D198" s="60" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E198" s="60"/>
       <c r="F198" s="60" t="s">
@@ -11056,13 +11056,13 @@
     </row>
     <row r="199" spans="1:13" s="5" customFormat="1" ht="2.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A199" s="5" t="s">
+        <v>425</v>
+      </c>
+      <c r="B199" s="5" t="s">
+        <v>425</v>
+      </c>
+      <c r="D199" s="5" t="s">
         <v>426</v>
-      </c>
-      <c r="B199" s="5" t="s">
-        <v>426</v>
-      </c>
-      <c r="D199" s="5" t="s">
-        <v>427</v>
       </c>
       <c r="F199" s="61" t="s">
         <v>41</v>
@@ -11079,16 +11079,16 @@
     </row>
     <row r="200" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A200" s="29" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B200" s="29" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="D200" s="29" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="F200" s="29" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G200" s="64" t="b">
         <v>1</v>
@@ -11102,16 +11102,16 @@
     </row>
     <row r="201" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A201" s="29" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B201" s="29" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="D201" s="29" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="F201" s="29" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="G201" s="64" t="b">
         <v>1</v>
@@ -11125,16 +11125,16 @@
     </row>
     <row r="202" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A202" s="29" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B202" s="29" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="D202" s="29" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="F202" s="29" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G202" s="64" t="b">
         <v>1</v>
@@ -11148,16 +11148,16 @@
     </row>
     <row r="203" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A203" s="29" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B203" s="29" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="D203" s="29" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="F203" s="29" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="G203" s="64" t="b">
         <v>1</v>
@@ -11171,16 +11171,16 @@
     </row>
     <row r="204" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A204" s="29" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B204" s="29" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="D204" s="29" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="F204" s="29" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="G204" s="64" t="b">
         <v>1</v>
@@ -11194,16 +11194,16 @@
     </row>
     <row r="205" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A205" s="29" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B205" s="29" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="D205" s="29" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="F205" s="29" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="G205" s="64" t="b">
         <v>1</v>
@@ -11217,16 +11217,16 @@
     </row>
     <row r="206" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A206" s="29" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B206" s="29" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="D206" s="29" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="F206" s="29" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="G206" s="64" t="b">
         <v>1</v>
@@ -11240,16 +11240,16 @@
     </row>
     <row r="207" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A207" s="29" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B207" s="29" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D207" s="29" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="F207" s="29" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="G207" s="64" t="b">
         <v>1</v>
@@ -11263,16 +11263,16 @@
     </row>
     <row r="208" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A208" s="29" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B208" s="29" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D208" s="29" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="F208" s="29" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="G208" s="64" t="b">
         <v>1</v>
@@ -11286,16 +11286,16 @@
     </row>
     <row r="209" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A209" s="29" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B209" s="29" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="D209" s="29" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="F209" s="29" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="G209" s="64" t="b">
         <v>1</v>
@@ -11309,16 +11309,16 @@
     </row>
     <row r="210" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A210" s="29" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B210" s="29" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="D210" s="29" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="F210" s="29" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="G210" s="64" t="b">
         <v>1</v>
@@ -11332,16 +11332,16 @@
     </row>
     <row r="211" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A211" s="29" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B211" s="29" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D211" s="29" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="F211" s="29" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="G211" s="64" t="b">
         <v>1</v>
@@ -11355,16 +11355,16 @@
     </row>
     <row r="212" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A212" s="29" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B212" s="29" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="D212" s="29" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="F212" s="29" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="G212" s="64" t="b">
         <v>1</v>
@@ -11378,16 +11378,16 @@
     </row>
     <row r="213" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A213" s="29" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B213" s="29" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D213" s="29" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="F213" s="29" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G213" s="64" t="b">
         <v>1</v>
@@ -11401,16 +11401,16 @@
     </row>
     <row r="214" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A214" s="29" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B214" s="29" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D214" s="29" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="F214" s="29" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="G214" s="64" t="b">
         <v>1</v>
@@ -11424,16 +11424,16 @@
     </row>
     <row r="215" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A215" s="29" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B215" s="29" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D215" s="29" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="F215" s="29" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="G215" s="64" t="b">
         <v>1</v>
@@ -11447,16 +11447,16 @@
     </row>
     <row r="216" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A216" s="29" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B216" s="29" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="D216" s="29" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="F216" s="29" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="G216" s="64" t="b">
         <v>1</v>
@@ -11470,16 +11470,16 @@
     </row>
     <row r="217" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A217" s="29" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B217" s="29" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="D217" s="29" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="F217" s="29" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="G217" s="64" t="b">
         <v>1</v>
@@ -11493,16 +11493,16 @@
     </row>
     <row r="218" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A218" s="29" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B218" s="29" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="D218" s="29" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="F218" s="29" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="G218" s="64" t="b">
         <v>1</v>
@@ -11516,16 +11516,16 @@
     </row>
     <row r="219" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A219" s="29" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B219" s="29" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="D219" s="29" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="F219" s="29" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="G219" s="64" t="b">
         <v>1</v>
@@ -11539,16 +11539,16 @@
     </row>
     <row r="220" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A220" s="29" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B220" s="29" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="D220" s="29" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="F220" s="29" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="G220" s="64" t="b">
         <v>1</v>
@@ -11562,16 +11562,16 @@
     </row>
     <row r="221" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A221" s="29" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B221" s="29" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="D221" s="29" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="F221" s="29" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="G221" s="64" t="b">
         <v>1</v>
@@ -11585,16 +11585,16 @@
     </row>
     <row r="222" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A222" s="29" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B222" s="29" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="D222" s="29" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="F222" s="29" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="G222" s="64" t="b">
         <v>1</v>
@@ -11608,16 +11608,16 @@
     </row>
     <row r="223" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A223" s="29" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B223" s="29" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="D223" s="29" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="F223" s="29" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="G223" s="64" t="b">
         <v>1</v>
@@ -11631,16 +11631,16 @@
     </row>
     <row r="224" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A224" s="29" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B224" s="29" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="D224" s="29" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="F224" s="29" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="G224" s="64" t="b">
         <v>1</v>
@@ -11654,16 +11654,16 @@
     </row>
     <row r="225" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A225" s="29" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B225" s="29" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="D225" s="29" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="F225" s="29" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="G225" s="64" t="b">
         <v>1</v>
@@ -11677,16 +11677,16 @@
     </row>
     <row r="226" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A226" s="29" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B226" s="29" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="D226" s="29" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="F226" s="29" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="G226" s="64" t="b">
         <v>1</v>
@@ -11700,16 +11700,16 @@
     </row>
     <row r="227" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A227" s="29" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B227" s="29" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="D227" s="29" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="F227" s="29" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="G227" s="64" t="b">
         <v>1</v>
@@ -11723,16 +11723,16 @@
     </row>
     <row r="228" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A228" s="29" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B228" s="29" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="D228" s="29" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="F228" s="29" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="G228" s="64" t="b">
         <v>1</v>
@@ -11746,16 +11746,16 @@
     </row>
     <row r="229" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A229" s="29" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B229" s="29" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="D229" s="29" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="F229" s="29" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="G229" s="64" t="b">
         <v>1</v>
@@ -11769,16 +11769,16 @@
     </row>
     <row r="230" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A230" s="29" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B230" s="29" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="D230" s="29" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="F230" s="29" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="G230" s="64" t="b">
         <v>1</v>
@@ -11792,16 +11792,16 @@
     </row>
     <row r="231" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A231" s="29" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B231" s="29" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="D231" s="29" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="F231" s="29" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="G231" s="64" t="b">
         <v>1</v>
@@ -11815,16 +11815,16 @@
     </row>
     <row r="232" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A232" s="29" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B232" s="29" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="D232" s="29" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="F232" s="29" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="G232" s="64" t="b">
         <v>1</v>
@@ -11838,16 +11838,16 @@
     </row>
     <row r="233" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A233" s="29" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B233" s="29" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="D233" s="29" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="F233" s="29" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="G233" s="64" t="b">
         <v>1</v>
@@ -11861,16 +11861,16 @@
     </row>
     <row r="234" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A234" s="29" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B234" s="29" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="D234" s="29" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="F234" s="29" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="G234" s="64" t="b">
         <v>1</v>
@@ -11884,16 +11884,16 @@
     </row>
     <row r="235" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A235" s="29" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B235" s="29" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="D235" s="29" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="F235" s="29" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="G235" s="64" t="b">
         <v>1</v>
@@ -11907,16 +11907,16 @@
     </row>
     <row r="236" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A236" s="29" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B236" s="29" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="D236" s="29" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="F236" s="29" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="G236" s="64" t="b">
         <v>1</v>
@@ -11930,16 +11930,16 @@
     </row>
     <row r="237" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A237" s="29" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B237" s="29" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="D237" s="29" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="F237" s="29" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="G237" s="64" t="b">
         <v>1</v>
@@ -11953,16 +11953,16 @@
     </row>
     <row r="238" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A238" s="29" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B238" s="29" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="D238" s="29" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="F238" s="29" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="G238" s="64" t="b">
         <v>1</v>
@@ -11976,16 +11976,16 @@
     </row>
     <row r="239" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A239" s="29" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B239" s="29" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="D239" s="29" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="F239" s="29" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="G239" s="64" t="b">
         <v>1</v>
@@ -11999,16 +11999,16 @@
     </row>
     <row r="240" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A240" s="29" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B240" s="29" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="D240" s="29" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="F240" s="29" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="G240" s="64" t="b">
         <v>1</v>
@@ -12022,16 +12022,16 @@
     </row>
     <row r="241" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A241" s="29" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B241" s="29" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="D241" s="29" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="F241" s="29" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="G241" s="64" t="b">
         <v>1</v>
@@ -12045,16 +12045,16 @@
     </row>
     <row r="242" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A242" s="29" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B242" s="29" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="D242" s="29" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="F242" s="29" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="G242" s="64" t="b">
         <v>1</v>
@@ -12068,16 +12068,16 @@
     </row>
     <row r="243" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A243" s="29" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B243" s="29" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="D243" s="29" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="F243" s="29" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="G243" s="64" t="b">
         <v>1</v>
@@ -12091,16 +12091,16 @@
     </row>
     <row r="244" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A244" s="29" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="B244" s="29" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="D244" s="29" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="F244" s="29" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="G244" s="64" t="b">
         <v>1</v>
@@ -12114,16 +12114,16 @@
     </row>
     <row r="245" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A245" s="29" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B245" s="29" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="D245" s="29" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="F245" s="29" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G245" s="64" t="b">
         <v>1</v>
@@ -12137,16 +12137,16 @@
     </row>
     <row r="246" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A246" s="29" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B246" s="29" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="D246" s="29" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="F246" s="29" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="G246" s="64" t="b">
         <v>1</v>
@@ -12160,16 +12160,16 @@
     </row>
     <row r="247" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A247" s="29" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B247" s="29" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="D247" s="29" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="F247" s="29" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="G247" s="64" t="b">
         <v>1</v>
@@ -12183,16 +12183,16 @@
     </row>
     <row r="248" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A248" s="29" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B248" s="29" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="D248" s="29" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="F248" s="29" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="G248" s="64" t="b">
         <v>1</v>
@@ -12206,16 +12206,16 @@
     </row>
     <row r="249" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A249" s="29" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B249" s="29" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="D249" s="29" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="F249" s="29" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="G249" s="64" t="b">
         <v>1</v>
@@ -12229,16 +12229,16 @@
     </row>
     <row r="250" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A250" s="29" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B250" s="29" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="D250" s="29" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="F250" s="29" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="G250" s="64" t="b">
         <v>1</v>
@@ -12252,16 +12252,16 @@
     </row>
     <row r="251" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A251" s="29" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B251" s="29" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="D251" s="29" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="F251" s="29" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="G251" s="64" t="b">
         <v>1</v>
@@ -12275,16 +12275,16 @@
     </row>
     <row r="252" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A252" s="29" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="B252" s="29" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="D252" s="29" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="F252" s="29" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="G252" s="64" t="b">
         <v>1</v>
@@ -12298,16 +12298,16 @@
     </row>
     <row r="253" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A253" s="29" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B253" s="29" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D253" s="29" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="F253" s="29" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="G253" s="64" t="b">
         <v>1</v>
@@ -12321,16 +12321,16 @@
     </row>
     <row r="254" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A254" s="29" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B254" s="29" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="D254" s="29" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="F254" s="29" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="G254" s="64" t="b">
         <v>1</v>
@@ -12344,16 +12344,16 @@
     </row>
     <row r="255" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A255" s="29" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B255" s="29" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="D255" s="29" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F255" s="29" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="G255" s="64" t="b">
         <v>1</v>
@@ -12367,16 +12367,16 @@
     </row>
     <row r="256" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A256" s="29" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B256" s="29" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="D256" s="29" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="F256" s="29" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="G256" s="64" t="b">
         <v>1</v>
@@ -12390,16 +12390,16 @@
     </row>
     <row r="257" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A257" s="29" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B257" s="29" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="D257" s="29" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="F257" s="29" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="G257" s="64" t="b">
         <v>1</v>
@@ -12413,16 +12413,16 @@
     </row>
     <row r="258" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A258" s="29" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B258" s="29" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D258" s="29" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="F258" s="29" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="G258" s="64" t="b">
         <v>1</v>
@@ -12436,16 +12436,16 @@
     </row>
     <row r="259" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A259" s="29" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="B259" s="29" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D259" s="29" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="F259" s="29" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="G259" s="64" t="b">
         <v>1</v>
@@ -12459,16 +12459,16 @@
     </row>
     <row r="260" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A260" s="29" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="B260" s="29" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="D260" s="29" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="F260" s="29" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="G260" s="64" t="b">
         <v>1</v>
@@ -12482,16 +12482,16 @@
     </row>
     <row r="261" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A261" s="29" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B261" s="29" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="D261" s="29" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="F261" s="29" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="G261" s="64" t="b">
         <v>1</v>
@@ -12505,16 +12505,16 @@
     </row>
     <row r="262" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A262" s="29" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="B262" s="29" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D262" s="29" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="F262" s="29" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="G262" s="64" t="b">
         <v>1</v>
@@ -12528,16 +12528,16 @@
     </row>
     <row r="263" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A263" s="29" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="B263" s="29" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="D263" s="29" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="F263" s="29" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="G263" s="64" t="b">
         <v>1</v>
@@ -12551,16 +12551,16 @@
     </row>
     <row r="264" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A264" s="29" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="B264" s="29" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="D264" s="29" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="F264" s="29" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="G264" s="64" t="b">
         <v>1</v>
@@ -12574,16 +12574,16 @@
     </row>
     <row r="265" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A265" s="29" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="B265" s="29" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="D265" s="29" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="F265" s="29" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="G265" s="64" t="b">
         <v>1</v>
@@ -12597,16 +12597,16 @@
     </row>
     <row r="266" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A266" s="29" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B266" s="29" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="D266" s="29" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F266" s="29" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="G266" s="64" t="b">
         <v>1</v>
@@ -12620,16 +12620,16 @@
     </row>
     <row r="267" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A267" s="29" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="B267" s="29" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="D267" s="29" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="F267" s="29" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="G267" s="64" t="b">
         <v>1</v>
@@ -12643,13 +12643,13 @@
     </row>
     <row r="268" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A268" s="29" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B268" s="29" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="D268" s="29" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="G268" s="64" t="b">
         <v>1</v>
@@ -12663,16 +12663,16 @@
     </row>
     <row r="269" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A269" s="29" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B269" s="29" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="D269" s="29" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="F269" s="29" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="G269" s="64" t="b">
         <v>1</v>
@@ -12686,16 +12686,16 @@
     </row>
     <row r="270" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A270" s="29" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="B270" s="29" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D270" s="29" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F270" s="29" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="G270" s="64" t="b">
         <v>1</v>
@@ -12709,16 +12709,16 @@
     </row>
     <row r="271" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A271" s="29" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B271" s="29" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="D271" s="29" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="F271" s="29" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="G271" s="64" t="b">
         <v>1</v>
@@ -12732,16 +12732,16 @@
     </row>
     <row r="272" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A272" s="29" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="B272" s="29" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="D272" s="29" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="F272" s="29" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="G272" s="64" t="b">
         <v>1</v>
@@ -12755,16 +12755,16 @@
     </row>
     <row r="273" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A273" s="29" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="B273" s="29" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="D273" s="29" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="F273" s="29" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="G273" s="64" t="b">
         <v>1</v>
@@ -12778,16 +12778,16 @@
     </row>
     <row r="274" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A274" s="29" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B274" s="29" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="D274" s="29" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="F274" s="29" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="G274" s="64" t="b">
         <v>1</v>
@@ -12801,16 +12801,16 @@
     </row>
     <row r="275" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A275" s="29" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B275" s="29" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="D275" s="29" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="F275" s="29" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="G275" s="64" t="b">
         <v>1</v>
@@ -12824,16 +12824,16 @@
     </row>
     <row r="276" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A276" s="29" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B276" s="29" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="D276" s="29" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="F276" s="29" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="G276" s="64" t="b">
         <v>1</v>
@@ -12847,16 +12847,16 @@
     </row>
     <row r="277" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A277" s="29" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="B277" s="29" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="D277" s="29" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="F277" s="29" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="G277" s="64" t="b">
         <v>1</v>
@@ -12870,16 +12870,16 @@
     </row>
     <row r="278" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A278" s="29" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="B278" s="29" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="D278" s="29" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="F278" s="29" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="G278" s="64" t="b">
         <v>1</v>
@@ -12893,16 +12893,16 @@
     </row>
     <row r="279" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A279" s="29" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="B279" s="29" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="D279" s="29" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="F279" s="29" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="G279" s="64" t="b">
         <v>1</v>
@@ -12916,16 +12916,16 @@
     </row>
     <row r="280" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A280" s="29" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="B280" s="29" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="D280" s="29" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="F280" s="29" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="G280" s="64" t="b">
         <v>1</v>
@@ -12939,16 +12939,16 @@
     </row>
     <row r="281" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A281" s="29" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="B281" s="29" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="D281" s="29" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="F281" s="29" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="G281" s="64" t="b">
         <v>1</v>
@@ -12962,16 +12962,16 @@
     </row>
     <row r="282" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A282" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="B282" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="D282" s="29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="F282" s="29" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="G282" s="64" t="b">
         <v>1</v>
@@ -12985,19 +12985,19 @@
     </row>
     <row r="283" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A283" s="29" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="B283" s="29" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="C283" s="29" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="D283" s="29" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="F283" s="29" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="G283" s="64" t="b">
         <v>1</v>
@@ -13536,15 +13536,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="67" t="s">
+        <v>525</v>
+      </c>
+      <c r="B1" t="s">
         <v>526</v>
-      </c>
-      <c r="B1" t="s">
-        <v>527</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="67" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="B2" t="s">
         <v>231</v>
@@ -13555,106 +13555,106 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="67" t="s">
+        <v>528</v>
+      </c>
+      <c r="B4" t="s">
         <v>529</v>
-      </c>
-      <c r="B4" t="s">
-        <v>530</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="67" t="s">
+        <v>530</v>
+      </c>
+      <c r="B5" t="s">
         <v>531</v>
-      </c>
-      <c r="B5" t="s">
-        <v>532</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="67" t="s">
+        <v>532</v>
+      </c>
+      <c r="B6" t="s">
         <v>533</v>
-      </c>
-      <c r="B6" t="s">
-        <v>534</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="67" t="s">
+        <v>534</v>
+      </c>
+      <c r="B7" t="s">
         <v>535</v>
-      </c>
-      <c r="B7" t="s">
-        <v>536</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="67" t="s">
+        <v>536</v>
+      </c>
+      <c r="B8" t="s">
         <v>537</v>
-      </c>
-      <c r="B8" t="s">
-        <v>538</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="67" t="s">
+        <v>538</v>
+      </c>
+      <c r="B9" t="s">
         <v>539</v>
-      </c>
-      <c r="B9" t="s">
-        <v>540</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="67" t="s">
+        <v>540</v>
+      </c>
+      <c r="B10" t="s">
         <v>541</v>
-      </c>
-      <c r="B10" t="s">
-        <v>542</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="67" t="s">
+        <v>542</v>
+      </c>
+      <c r="B11" t="s">
         <v>543</v>
-      </c>
-      <c r="B11" t="s">
-        <v>544</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="67" t="s">
+        <v>544</v>
+      </c>
+      <c r="B12" t="s">
         <v>545</v>
-      </c>
-      <c r="B12" t="s">
-        <v>546</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="67" t="s">
+        <v>546</v>
+      </c>
+      <c r="B13" t="s">
         <v>547</v>
-      </c>
-      <c r="B13" t="s">
-        <v>548</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="67" t="s">
+        <v>548</v>
+      </c>
+      <c r="B14" t="s">
         <v>549</v>
-      </c>
-      <c r="B14" t="s">
-        <v>550</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="67" t="s">
+        <v>550</v>
+      </c>
+      <c r="B15" t="s">
         <v>551</v>
-      </c>
-      <c r="B15" t="s">
-        <v>552</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="67" t="s">
+        <v>552</v>
+      </c>
+      <c r="B16" t="s">
         <v>553</v>
-      </c>
-      <c r="B16" t="s">
-        <v>554</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -13665,7 +13665,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="67" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="B19" t="s">
         <v>232</v>

</xml_diff>

<commit_message>
Updated BTAPResults/measure.rb to include osm files.
</commit_message>
<xml_diff>
--- a/projects/NECB_Full_WeatherFile_Scan.xlsx
+++ b/projects/NECB_Full_WeatherFile_Scan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="5490" windowWidth="20370" windowHeight="5025" tabRatio="469" activeTab="2"/>
+    <workbookView xWindow="-15" yWindow="5490" windowWidth="20370" windowHeight="5025" tabRatio="469" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="9" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1103" uniqueCount="557">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1103" uniqueCount="558">
   <si>
     <t>type</t>
   </si>
@@ -732,9 +732,6 @@
     <t>["CAN_BC_Vancouver.718920_CWEC.epw","CAN_ON_Toronto.716240_CWEC.epw","CAN_PQ_Sherbrooke.716100_CWEC.epw","CAN_YT_Whitehorse.719640_CWEC.epw","CAN_NU_Resolute.719240_CWEC.epw"]</t>
   </si>
   <si>
-    <t>["FullServiceRestaurant","HighriseApartment","LargeHotel","LargeOffice","MediumOffice","MidriseApartment","Outpatient","PrimarySchool","QuickServiceRestaurant","RetailStandalone","SecondarySchool","SmallHotel","SmallOffice","RetailStripmall","Warehouse"]</t>
-  </si>
-  <si>
     <t>../../openstudio-standards/openstudio-standards/data/weather/CAN_BC_Vancouver.718920_CWEC.epw</t>
   </si>
   <si>
@@ -1708,6 +1705,12 @@
   </si>
   <si>
     <t>btapresults.total_utility_cost_intensity</t>
+  </si>
+  <si>
+    <t>["FullServiceRestaurant","'Hospital'","HighriseApartment","LargeHotel","LargeOffice","MediumOffice","MidriseApartment","Outpatient","PrimarySchool","QuickServiceRestaurant","RetailStandalone","SecondarySchool","SmallHotel","SmallOffice","RetailStripmall","Warehouse"]</t>
+  </si>
+  <si>
+    <t>["CAN_ON_Toronto.716240_CWEC.epw"]</t>
   </si>
 </sst>
 </file>
@@ -6603,7 +6606,7 @@
         <v>66</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>67</v>
@@ -6625,7 +6628,7 @@
         <v>78</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>80</v>
@@ -6696,7 +6699,7 @@
         <v>36</v>
       </c>
       <c r="B12" s="23" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>79</v>
@@ -6809,7 +6812,7 @@
         <v>62</v>
       </c>
       <c r="C23" s="44" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="D23" s="31" t="s">
         <v>62</v>
@@ -6890,7 +6893,7 @@
         <v>26</v>
       </c>
       <c r="B35" s="23" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -6907,7 +6910,7 @@
         <v>26</v>
       </c>
       <c r="B37" s="23" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D37" s="2"/>
     </row>
@@ -6916,7 +6919,7 @@
         <v>26</v>
       </c>
       <c r="B38" s="23" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D38" s="2"/>
     </row>
@@ -6925,7 +6928,7 @@
         <v>26</v>
       </c>
       <c r="B39" s="23" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D39" s="2"/>
     </row>
@@ -7009,8 +7012,8 @@
   </sheetPr>
   <dimension ref="A1:Z10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -7221,7 +7224,7 @@
         <v>1</v>
       </c>
       <c r="P5" s="44" t="s">
-        <v>231</v>
+        <v>556</v>
       </c>
       <c r="R5" s="50" t="s">
         <v>214</v>
@@ -7338,7 +7341,7 @@
         <v>1</v>
       </c>
       <c r="P8" s="44" t="s">
-        <v>230</v>
+        <v>557</v>
       </c>
       <c r="R8" s="50" t="s">
         <v>214</v>
@@ -7349,16 +7352,16 @@
         <v>1</v>
       </c>
       <c r="B9" s="58" t="s">
+        <v>415</v>
+      </c>
+      <c r="C9" s="58" t="s">
+        <v>415</v>
+      </c>
+      <c r="D9" s="58" t="s">
+        <v>415</v>
+      </c>
+      <c r="E9" s="65" t="s">
         <v>416</v>
-      </c>
-      <c r="C9" s="58" t="s">
-        <v>416</v>
-      </c>
-      <c r="D9" s="58" t="s">
-        <v>416</v>
-      </c>
-      <c r="E9" s="65" t="s">
-        <v>417</v>
       </c>
       <c r="I9" s="59"/>
       <c r="J9" s="59"/>
@@ -7368,16 +7371,16 @@
         <v>0</v>
       </c>
       <c r="B10" s="49" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C10" s="49" t="s">
+        <v>236</v>
+      </c>
+      <c r="D10" s="49" t="s">
         <v>237</v>
       </c>
-      <c r="D10" s="49" t="s">
-        <v>238</v>
-      </c>
       <c r="E10" s="49" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="I10" s="46"/>
       <c r="J10" s="46"/>
@@ -8010,10 +8013,10 @@
     </row>
     <row r="21" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="18" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D21" s="18" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="G21" s="57" t="b">
         <v>1</v>
@@ -8027,10 +8030,10 @@
     </row>
     <row r="22" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="18" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D22" s="18" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G22" s="57" t="b">
         <v>1</v>
@@ -8044,10 +8047,10 @@
     </row>
     <row r="23" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="18" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D23" s="18" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G23" s="57" t="b">
         <v>1</v>
@@ -8061,10 +8064,10 @@
     </row>
     <row r="24" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="18" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D24" s="18" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G24" s="57" t="b">
         <v>1</v>
@@ -8078,10 +8081,10 @@
     </row>
     <row r="25" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="18" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D25" s="18" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G25" s="57" t="b">
         <v>1</v>
@@ -8095,10 +8098,10 @@
     </row>
     <row r="26" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="18" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D26" s="18" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G26" s="57" t="b">
         <v>1</v>
@@ -8112,10 +8115,10 @@
     </row>
     <row r="27" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="18" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D27" s="18" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G27" s="57" t="b">
         <v>1</v>
@@ -8129,10 +8132,10 @@
     </row>
     <row r="28" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="18" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D28" s="18" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G28" s="57" t="b">
         <v>1</v>
@@ -8146,10 +8149,10 @@
     </row>
     <row r="29" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="18" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D29" s="18" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G29" s="57" t="b">
         <v>1</v>
@@ -8163,10 +8166,10 @@
     </row>
     <row r="30" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="18" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D30" s="18" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="G30" s="57" t="b">
         <v>1</v>
@@ -8180,10 +8183,10 @@
     </row>
     <row r="31" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="18" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D31" s="18" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G31" s="57" t="b">
         <v>1</v>
@@ -8197,10 +8200,10 @@
     </row>
     <row r="32" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="18" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D32" s="18" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G32" s="57" t="b">
         <v>1</v>
@@ -8214,10 +8217,10 @@
     </row>
     <row r="33" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="18" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D33" s="18" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="G33" s="57" t="b">
         <v>1</v>
@@ -8231,10 +8234,10 @@
     </row>
     <row r="34" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="18" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D34" s="18" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="G34" s="57" t="b">
         <v>1</v>
@@ -8248,10 +8251,10 @@
     </row>
     <row r="35" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="18" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D35" s="18" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="G35" s="57" t="b">
         <v>1</v>
@@ -8265,10 +8268,10 @@
     </row>
     <row r="36" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="18" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D36" s="18" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="G36" s="57" t="b">
         <v>1</v>
@@ -8282,10 +8285,10 @@
     </row>
     <row r="37" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="18" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D37" s="18" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G37" s="57" t="b">
         <v>1</v>
@@ -8299,10 +8302,10 @@
     </row>
     <row r="38" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="18" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D38" s="18" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G38" s="57" t="b">
         <v>1</v>
@@ -8316,10 +8319,10 @@
     </row>
     <row r="39" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="18" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D39" s="18" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="G39" s="57" t="b">
         <v>1</v>
@@ -8333,10 +8336,10 @@
     </row>
     <row r="40" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="18" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D40" s="18" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="G40" s="57" t="b">
         <v>1</v>
@@ -8350,10 +8353,10 @@
     </row>
     <row r="41" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="18" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D41" s="18" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="G41" s="57" t="b">
         <v>1</v>
@@ -8367,10 +8370,10 @@
     </row>
     <row r="42" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="18" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D42" s="18" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="G42" s="57" t="b">
         <v>1</v>
@@ -8384,10 +8387,10 @@
     </row>
     <row r="43" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="18" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D43" s="18" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="G43" s="57" t="b">
         <v>1</v>
@@ -8401,10 +8404,10 @@
     </row>
     <row r="44" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="18" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D44" s="18" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="G44" s="57" t="b">
         <v>1</v>
@@ -8418,10 +8421,10 @@
     </row>
     <row r="45" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="18" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D45" s="18" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="G45" s="57" t="b">
         <v>1</v>
@@ -8435,10 +8438,10 @@
     </row>
     <row r="46" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="18" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D46" s="18" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="G46" s="57" t="b">
         <v>1</v>
@@ -8452,10 +8455,10 @@
     </row>
     <row r="47" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="18" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D47" s="18" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="G47" s="57" t="b">
         <v>1</v>
@@ -8469,10 +8472,10 @@
     </row>
     <row r="48" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="18" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D48" s="18" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="G48" s="57" t="b">
         <v>1</v>
@@ -8486,10 +8489,10 @@
     </row>
     <row r="49" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="18" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D49" s="18" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="G49" s="57" t="b">
         <v>1</v>
@@ -8503,10 +8506,10 @@
     </row>
     <row r="50" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="18" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D50" s="18" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="G50" s="57" t="b">
         <v>1</v>
@@ -8520,10 +8523,10 @@
     </row>
     <row r="51" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="18" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D51" s="18" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="G51" s="57" t="b">
         <v>1</v>
@@ -8537,10 +8540,10 @@
     </row>
     <row r="52" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="18" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D52" s="18" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="G52" s="57" t="b">
         <v>1</v>
@@ -8554,10 +8557,10 @@
     </row>
     <row r="53" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="18" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D53" s="18" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="G53" s="57" t="b">
         <v>1</v>
@@ -8571,10 +8574,10 @@
     </row>
     <row r="54" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="18" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D54" s="18" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="G54" s="57" t="b">
         <v>1</v>
@@ -8588,10 +8591,10 @@
     </row>
     <row r="55" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="18" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D55" s="18" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="G55" s="57" t="b">
         <v>1</v>
@@ -8605,10 +8608,10 @@
     </row>
     <row r="56" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="18" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D56" s="18" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="G56" s="57" t="b">
         <v>1</v>
@@ -8622,10 +8625,10 @@
     </row>
     <row r="57" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="18" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D57" s="18" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="G57" s="57" t="b">
         <v>1</v>
@@ -8639,10 +8642,10 @@
     </row>
     <row r="58" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="18" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D58" s="18" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="G58" s="57" t="b">
         <v>1</v>
@@ -8656,10 +8659,10 @@
     </row>
     <row r="59" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="18" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D59" s="18" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G59" s="57" t="b">
         <v>1</v>
@@ -8673,10 +8676,10 @@
     </row>
     <row r="60" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="18" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D60" s="18" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G60" s="57" t="b">
         <v>1</v>
@@ -8690,10 +8693,10 @@
     </row>
     <row r="61" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="18" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D61" s="18" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G61" s="57" t="b">
         <v>1</v>
@@ -8707,10 +8710,10 @@
     </row>
     <row r="62" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="18" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D62" s="18" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="G62" s="57" t="b">
         <v>1</v>
@@ -8724,10 +8727,10 @@
     </row>
     <row r="63" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="18" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D63" s="18" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="G63" s="57" t="b">
         <v>1</v>
@@ -8741,10 +8744,10 @@
     </row>
     <row r="64" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="18" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D64" s="18" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="G64" s="57" t="b">
         <v>1</v>
@@ -8758,10 +8761,10 @@
     </row>
     <row r="65" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="18" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D65" s="18" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G65" s="57" t="b">
         <v>1</v>
@@ -8775,10 +8778,10 @@
     </row>
     <row r="66" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="18" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D66" s="18" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="G66" s="57" t="b">
         <v>1</v>
@@ -8792,10 +8795,10 @@
     </row>
     <row r="67" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="18" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D67" s="18" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="G67" s="57" t="b">
         <v>1</v>
@@ -8809,10 +8812,10 @@
     </row>
     <row r="68" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="18" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D68" s="18" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="G68" s="57" t="b">
         <v>1</v>
@@ -8826,10 +8829,10 @@
     </row>
     <row r="69" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="18" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D69" s="18" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="G69" s="57" t="b">
         <v>1</v>
@@ -8843,10 +8846,10 @@
     </row>
     <row r="70" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="18" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D70" s="18" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="G70" s="57" t="b">
         <v>1</v>
@@ -8860,10 +8863,10 @@
     </row>
     <row r="71" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="18" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D71" s="18" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="G71" s="57" t="b">
         <v>1</v>
@@ -8877,10 +8880,10 @@
     </row>
     <row r="72" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="18" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D72" s="18" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="G72" s="57" t="b">
         <v>1</v>
@@ -8894,10 +8897,10 @@
     </row>
     <row r="73" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="18" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D73" s="18" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="G73" s="57" t="b">
         <v>1</v>
@@ -8911,10 +8914,10 @@
     </row>
     <row r="74" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="18" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D74" s="18" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="G74" s="57" t="b">
         <v>1</v>
@@ -8928,10 +8931,10 @@
     </row>
     <row r="75" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="18" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D75" s="18" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="G75" s="57" t="b">
         <v>1</v>
@@ -8945,10 +8948,10 @@
     </row>
     <row r="76" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="18" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D76" s="18" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="G76" s="57" t="b">
         <v>1</v>
@@ -8962,10 +8965,10 @@
     </row>
     <row r="77" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="18" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D77" s="18" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G77" s="57" t="b">
         <v>1</v>
@@ -8979,10 +8982,10 @@
     </row>
     <row r="78" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="18" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D78" s="18" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="G78" s="57" t="b">
         <v>1</v>
@@ -8996,10 +8999,10 @@
     </row>
     <row r="79" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="18" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D79" s="18" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="G79" s="57" t="b">
         <v>1</v>
@@ -9013,10 +9016,10 @@
     </row>
     <row r="80" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="18" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D80" s="18" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="G80" s="57" t="b">
         <v>1</v>
@@ -9030,10 +9033,10 @@
     </row>
     <row r="81" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="18" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D81" s="18" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="G81" s="57" t="b">
         <v>1</v>
@@ -9047,10 +9050,10 @@
     </row>
     <row r="82" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="18" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D82" s="18" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="G82" s="57" t="b">
         <v>1</v>
@@ -9064,10 +9067,10 @@
     </row>
     <row r="83" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="18" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D83" s="18" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="G83" s="57" t="b">
         <v>1</v>
@@ -9081,10 +9084,10 @@
     </row>
     <row r="84" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="18" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D84" s="18" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="G84" s="57" t="b">
         <v>1</v>
@@ -9098,10 +9101,10 @@
     </row>
     <row r="85" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="18" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D85" s="18" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="G85" s="57" t="b">
         <v>1</v>
@@ -9115,10 +9118,10 @@
     </row>
     <row r="86" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="18" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D86" s="18" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="G86" s="57" t="b">
         <v>1</v>
@@ -9132,10 +9135,10 @@
     </row>
     <row r="87" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="18" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D87" s="18" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="G87" s="57" t="b">
         <v>1</v>
@@ -9149,10 +9152,10 @@
     </row>
     <row r="88" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="18" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D88" s="18" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="G88" s="57" t="b">
         <v>1</v>
@@ -9166,10 +9169,10 @@
     </row>
     <row r="89" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="18" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D89" s="18" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="G89" s="57" t="b">
         <v>1</v>
@@ -9183,10 +9186,10 @@
     </row>
     <row r="90" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="18" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D90" s="18" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G90" s="57" t="b">
         <v>1</v>
@@ -9200,10 +9203,10 @@
     </row>
     <row r="91" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="18" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D91" s="18" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="G91" s="57" t="b">
         <v>1</v>
@@ -9217,10 +9220,10 @@
     </row>
     <row r="92" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="18" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D92" s="18" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="G92" s="57" t="b">
         <v>1</v>
@@ -9234,10 +9237,10 @@
     </row>
     <row r="93" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="18" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D93" s="18" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="G93" s="57" t="b">
         <v>1</v>
@@ -9251,10 +9254,10 @@
     </row>
     <row r="94" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A94" s="18" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D94" s="18" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="G94" s="57" t="b">
         <v>1</v>
@@ -9268,10 +9271,10 @@
     </row>
     <row r="95" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A95" s="18" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D95" s="18" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="G95" s="57" t="b">
         <v>1</v>
@@ -9285,10 +9288,10 @@
     </row>
     <row r="96" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A96" s="18" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D96" s="18" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="G96" s="57" t="b">
         <v>1</v>
@@ -9302,10 +9305,10 @@
     </row>
     <row r="97" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A97" s="18" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D97" s="18" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="G97" s="57" t="b">
         <v>1</v>
@@ -9319,10 +9322,10 @@
     </row>
     <row r="98" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98" s="18" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D98" s="18" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="G98" s="57" t="b">
         <v>1</v>
@@ -9336,10 +9339,10 @@
     </row>
     <row r="99" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A99" s="18" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D99" s="18" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="G99" s="57" t="b">
         <v>1</v>
@@ -9353,10 +9356,10 @@
     </row>
     <row r="100" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A100" s="18" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D100" s="18" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="G100" s="57" t="b">
         <v>1</v>
@@ -9370,10 +9373,10 @@
     </row>
     <row r="101" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A101" s="18" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D101" s="18" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="G101" s="57" t="b">
         <v>1</v>
@@ -9387,10 +9390,10 @@
     </row>
     <row r="102" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A102" s="18" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D102" s="18" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="G102" s="57" t="b">
         <v>1</v>
@@ -9404,10 +9407,10 @@
     </row>
     <row r="103" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A103" s="18" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D103" s="18" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="G103" s="57" t="b">
         <v>1</v>
@@ -9421,10 +9424,10 @@
     </row>
     <row r="104" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A104" s="18" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D104" s="18" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="G104" s="57" t="b">
         <v>1</v>
@@ -9438,10 +9441,10 @@
     </row>
     <row r="105" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A105" s="18" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D105" s="18" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="G105" s="57" t="b">
         <v>1</v>
@@ -9455,10 +9458,10 @@
     </row>
     <row r="106" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A106" s="18" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D106" s="18" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="G106" s="57" t="b">
         <v>1</v>
@@ -9472,10 +9475,10 @@
     </row>
     <row r="107" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A107" s="18" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D107" s="18" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="G107" s="57" t="b">
         <v>1</v>
@@ -9489,10 +9492,10 @@
     </row>
     <row r="108" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A108" s="18" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D108" s="18" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G108" s="57" t="b">
         <v>1</v>
@@ -9506,10 +9509,10 @@
     </row>
     <row r="109" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A109" s="18" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D109" s="18" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="G109" s="57" t="b">
         <v>1</v>
@@ -9523,10 +9526,10 @@
     </row>
     <row r="110" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A110" s="18" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D110" s="18" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="G110" s="57" t="b">
         <v>1</v>
@@ -9540,10 +9543,10 @@
     </row>
     <row r="111" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A111" s="18" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D111" s="18" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="G111" s="57" t="b">
         <v>1</v>
@@ -9557,10 +9560,10 @@
     </row>
     <row r="112" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A112" s="18" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D112" s="18" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G112" s="57" t="b">
         <v>1</v>
@@ -9574,10 +9577,10 @@
     </row>
     <row r="113" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A113" s="18" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D113" s="18" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="G113" s="57" t="b">
         <v>1</v>
@@ -9591,10 +9594,10 @@
     </row>
     <row r="114" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A114" s="18" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D114" s="18" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="G114" s="57" t="b">
         <v>1</v>
@@ -9608,10 +9611,10 @@
     </row>
     <row r="115" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A115" s="18" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D115" s="18" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G115" s="57" t="b">
         <v>1</v>
@@ -9625,10 +9628,10 @@
     </row>
     <row r="116" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A116" s="18" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D116" s="18" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="G116" s="57" t="b">
         <v>1</v>
@@ -9642,10 +9645,10 @@
     </row>
     <row r="117" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A117" s="18" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D117" s="18" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G117" s="57" t="b">
         <v>1</v>
@@ -9659,10 +9662,10 @@
     </row>
     <row r="118" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A118" s="18" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="D118" s="18" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="G118" s="57" t="b">
         <v>1</v>
@@ -9676,10 +9679,10 @@
     </row>
     <row r="119" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A119" s="18" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="D119" s="18" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="G119" s="57" t="b">
         <v>1</v>
@@ -9693,10 +9696,10 @@
     </row>
     <row r="120" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A120" s="18" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D120" s="18" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="G120" s="57" t="b">
         <v>1</v>
@@ -9710,10 +9713,10 @@
     </row>
     <row r="121" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A121" s="18" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D121" s="18" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="G121" s="57" t="b">
         <v>1</v>
@@ -9727,10 +9730,10 @@
     </row>
     <row r="122" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A122" s="18" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D122" s="18" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G122" s="57" t="b">
         <v>1</v>
@@ -9744,10 +9747,10 @@
     </row>
     <row r="123" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A123" s="18" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D123" s="18" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G123" s="57" t="b">
         <v>1</v>
@@ -9761,10 +9764,10 @@
     </row>
     <row r="124" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A124" s="18" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D124" s="18" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="G124" s="57" t="b">
         <v>1</v>
@@ -9778,10 +9781,10 @@
     </row>
     <row r="125" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A125" s="18" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D125" s="18" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="G125" s="57" t="b">
         <v>1</v>
@@ -9795,10 +9798,10 @@
     </row>
     <row r="126" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A126" s="18" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D126" s="18" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="G126" s="57" t="b">
         <v>1</v>
@@ -9812,10 +9815,10 @@
     </row>
     <row r="127" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A127" s="18" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D127" s="18" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="G127" s="57" t="b">
         <v>1</v>
@@ -9829,10 +9832,10 @@
     </row>
     <row r="128" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A128" s="18" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D128" s="18" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="G128" s="57" t="b">
         <v>1</v>
@@ -9846,10 +9849,10 @@
     </row>
     <row r="129" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A129" s="18" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D129" s="18" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="G129" s="57" t="b">
         <v>1</v>
@@ -9863,10 +9866,10 @@
     </row>
     <row r="130" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A130" s="18" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D130" s="18" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="G130" s="57" t="b">
         <v>1</v>
@@ -9880,10 +9883,10 @@
     </row>
     <row r="131" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A131" s="18" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D131" s="18" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="G131" s="57" t="b">
         <v>1</v>
@@ -9897,10 +9900,10 @@
     </row>
     <row r="132" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A132" s="18" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D132" s="18" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="G132" s="57" t="b">
         <v>1</v>
@@ -9914,10 +9917,10 @@
     </row>
     <row r="133" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A133" s="18" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D133" s="18" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="G133" s="57" t="b">
         <v>1</v>
@@ -9931,10 +9934,10 @@
     </row>
     <row r="134" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A134" s="18" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D134" s="18" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="G134" s="57" t="b">
         <v>1</v>
@@ -9948,10 +9951,10 @@
     </row>
     <row r="135" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A135" s="18" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D135" s="18" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G135" s="57" t="b">
         <v>1</v>
@@ -9965,10 +9968,10 @@
     </row>
     <row r="136" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A136" s="18" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D136" s="18" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="G136" s="57" t="b">
         <v>1</v>
@@ -9982,10 +9985,10 @@
     </row>
     <row r="137" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A137" s="18" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="D137" s="18" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="G137" s="57" t="b">
         <v>1</v>
@@ -9999,10 +10002,10 @@
     </row>
     <row r="138" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A138" s="18" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="D138" s="18" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="G138" s="57" t="b">
         <v>1</v>
@@ -10016,10 +10019,10 @@
     </row>
     <row r="139" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A139" s="18" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D139" s="18" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="G139" s="57" t="b">
         <v>1</v>
@@ -10033,10 +10036,10 @@
     </row>
     <row r="140" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A140" s="18" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D140" s="18" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="G140" s="57" t="b">
         <v>1</v>
@@ -10050,10 +10053,10 @@
     </row>
     <row r="141" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A141" s="18" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D141" s="18" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="G141" s="57" t="b">
         <v>1</v>
@@ -10067,10 +10070,10 @@
     </row>
     <row r="142" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A142" s="18" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="D142" s="18" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="G142" s="57" t="b">
         <v>1</v>
@@ -10084,10 +10087,10 @@
     </row>
     <row r="143" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A143" s="18" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D143" s="18" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="G143" s="57" t="b">
         <v>1</v>
@@ -10101,10 +10104,10 @@
     </row>
     <row r="144" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A144" s="18" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D144" s="18" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="G144" s="57" t="b">
         <v>1</v>
@@ -10118,10 +10121,10 @@
     </row>
     <row r="145" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A145" s="18" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D145" s="18" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="G145" s="57" t="b">
         <v>1</v>
@@ -10135,10 +10138,10 @@
     </row>
     <row r="146" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A146" s="18" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="D146" s="18" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="G146" s="57" t="b">
         <v>1</v>
@@ -10152,10 +10155,10 @@
     </row>
     <row r="147" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A147" s="18" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="D147" s="18" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="G147" s="57" t="b">
         <v>1</v>
@@ -10169,10 +10172,10 @@
     </row>
     <row r="148" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A148" s="18" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D148" s="18" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="G148" s="57" t="b">
         <v>1</v>
@@ -10186,10 +10189,10 @@
     </row>
     <row r="149" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A149" s="18" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D149" s="18" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="G149" s="57" t="b">
         <v>1</v>
@@ -10203,10 +10206,10 @@
     </row>
     <row r="150" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A150" s="18" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D150" s="18" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="G150" s="57" t="b">
         <v>1</v>
@@ -10220,10 +10223,10 @@
     </row>
     <row r="151" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A151" s="18" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D151" s="18" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="G151" s="57" t="b">
         <v>1</v>
@@ -10237,10 +10240,10 @@
     </row>
     <row r="152" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A152" s="18" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D152" s="18" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="G152" s="57" t="b">
         <v>1</v>
@@ -10254,10 +10257,10 @@
     </row>
     <row r="153" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A153" s="18" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D153" s="18" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="G153" s="57" t="b">
         <v>1</v>
@@ -10271,10 +10274,10 @@
     </row>
     <row r="154" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A154" s="18" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D154" s="18" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="G154" s="57" t="b">
         <v>1</v>
@@ -10288,10 +10291,10 @@
     </row>
     <row r="155" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A155" s="18" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D155" s="18" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="G155" s="57" t="b">
         <v>1</v>
@@ -10305,10 +10308,10 @@
     </row>
     <row r="156" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A156" s="18" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D156" s="18" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="G156" s="57" t="b">
         <v>1</v>
@@ -10322,10 +10325,10 @@
     </row>
     <row r="157" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A157" s="18" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D157" s="18" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="G157" s="57" t="b">
         <v>1</v>
@@ -10339,10 +10342,10 @@
     </row>
     <row r="158" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A158" s="18" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="D158" s="18" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="G158" s="57" t="b">
         <v>1</v>
@@ -10356,10 +10359,10 @@
     </row>
     <row r="159" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A159" s="18" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D159" s="18" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="G159" s="57" t="b">
         <v>1</v>
@@ -10373,10 +10376,10 @@
     </row>
     <row r="160" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A160" s="18" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D160" s="18" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G160" s="57" t="b">
         <v>1</v>
@@ -10390,10 +10393,10 @@
     </row>
     <row r="161" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A161" s="18" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="D161" s="18" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="G161" s="57" t="b">
         <v>1</v>
@@ -10407,10 +10410,10 @@
     </row>
     <row r="162" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A162" s="18" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="D162" s="18" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="G162" s="57" t="b">
         <v>1</v>
@@ -10424,10 +10427,10 @@
     </row>
     <row r="163" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A163" s="18" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D163" s="18" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="G163" s="57" t="b">
         <v>1</v>
@@ -10441,10 +10444,10 @@
     </row>
     <row r="164" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A164" s="18" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="D164" s="18" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="G164" s="57" t="b">
         <v>1</v>
@@ -10458,10 +10461,10 @@
     </row>
     <row r="165" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A165" s="18" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D165" s="18" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="G165" s="57" t="b">
         <v>1</v>
@@ -10475,10 +10478,10 @@
     </row>
     <row r="166" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A166" s="18" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D166" s="18" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="G166" s="57" t="b">
         <v>1</v>
@@ -10492,10 +10495,10 @@
     </row>
     <row r="167" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A167" s="18" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D167" s="18" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="G167" s="57" t="b">
         <v>1</v>
@@ -10509,10 +10512,10 @@
     </row>
     <row r="168" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A168" s="18" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D168" s="18" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="G168" s="57" t="b">
         <v>1</v>
@@ -10526,10 +10529,10 @@
     </row>
     <row r="169" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A169" s="18" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D169" s="18" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="G169" s="57" t="b">
         <v>1</v>
@@ -10543,10 +10546,10 @@
     </row>
     <row r="170" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A170" s="18" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D170" s="18" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="G170" s="57" t="b">
         <v>1</v>
@@ -10560,10 +10563,10 @@
     </row>
     <row r="171" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A171" s="18" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="D171" s="18" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="G171" s="57" t="b">
         <v>1</v>
@@ -10577,10 +10580,10 @@
     </row>
     <row r="172" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A172" s="18" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="D172" s="18" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="G172" s="57" t="b">
         <v>1</v>
@@ -10594,10 +10597,10 @@
     </row>
     <row r="173" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A173" s="18" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D173" s="18" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="G173" s="57" t="b">
         <v>1</v>
@@ -10611,10 +10614,10 @@
     </row>
     <row r="174" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A174" s="18" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="D174" s="18" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="G174" s="57" t="b">
         <v>1</v>
@@ -10628,10 +10631,10 @@
     </row>
     <row r="175" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A175" s="18" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D175" s="18" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="G175" s="57" t="b">
         <v>1</v>
@@ -10645,10 +10648,10 @@
     </row>
     <row r="176" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A176" s="18" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D176" s="18" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="G176" s="57" t="b">
         <v>1</v>
@@ -10662,10 +10665,10 @@
     </row>
     <row r="177" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A177" s="18" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D177" s="18" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="G177" s="57" t="b">
         <v>1</v>
@@ -10679,10 +10682,10 @@
     </row>
     <row r="178" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A178" s="18" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D178" s="18" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="G178" s="57" t="b">
         <v>1</v>
@@ -10696,10 +10699,10 @@
     </row>
     <row r="179" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A179" s="18" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="D179" s="18" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="G179" s="57" t="b">
         <v>1</v>
@@ -10713,10 +10716,10 @@
     </row>
     <row r="180" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A180" s="18" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="D180" s="18" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="G180" s="57" t="b">
         <v>1</v>
@@ -10730,10 +10733,10 @@
     </row>
     <row r="181" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A181" s="18" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D181" s="18" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="G181" s="57" t="b">
         <v>1</v>
@@ -10747,10 +10750,10 @@
     </row>
     <row r="182" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A182" s="18" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D182" s="18" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="G182" s="57" t="b">
         <v>1</v>
@@ -10764,10 +10767,10 @@
     </row>
     <row r="183" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A183" s="18" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D183" s="18" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="G183" s="57" t="b">
         <v>1</v>
@@ -10781,10 +10784,10 @@
     </row>
     <row r="184" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A184" s="18" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D184" s="18" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="G184" s="57" t="b">
         <v>1</v>
@@ -10798,10 +10801,10 @@
     </row>
     <row r="185" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A185" s="18" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D185" s="18" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="G185" s="57" t="b">
         <v>1</v>
@@ -10815,10 +10818,10 @@
     </row>
     <row r="186" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A186" s="18" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="D186" s="18" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="G186" s="57" t="b">
         <v>1</v>
@@ -10832,10 +10835,10 @@
     </row>
     <row r="187" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A187" s="18" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="D187" s="18" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="G187" s="57" t="b">
         <v>1</v>
@@ -10849,10 +10852,10 @@
     </row>
     <row r="188" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A188" s="18" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="D188" s="18" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="G188" s="57" t="b">
         <v>1</v>
@@ -10866,10 +10869,10 @@
     </row>
     <row r="189" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A189" s="18" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="D189" s="18" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="G189" s="57" t="b">
         <v>1</v>
@@ -10883,10 +10886,10 @@
     </row>
     <row r="190" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A190" s="18" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="D190" s="18" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="G190" s="57" t="b">
         <v>1</v>
@@ -10900,10 +10903,10 @@
     </row>
     <row r="191" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A191" s="18" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D191" s="18" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="G191" s="57" t="b">
         <v>1</v>
@@ -10917,10 +10920,10 @@
     </row>
     <row r="192" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A192" s="18" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="D192" s="18" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="G192" s="57" t="b">
         <v>1</v>
@@ -10934,10 +10937,10 @@
     </row>
     <row r="193" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A193" s="18" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D193" s="18" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="G193" s="57" t="b">
         <v>1</v>
@@ -10951,10 +10954,10 @@
     </row>
     <row r="194" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A194" s="18" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D194" s="18" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="G194" s="57" t="b">
         <v>1</v>
@@ -10968,10 +10971,10 @@
     </row>
     <row r="195" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A195" s="18" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D195" s="18" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="G195" s="57" t="b">
         <v>1</v>
@@ -10985,10 +10988,10 @@
     </row>
     <row r="196" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A196" s="18" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="D196" s="18" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="G196" s="57" t="b">
         <v>1</v>
@@ -11002,10 +11005,10 @@
     </row>
     <row r="197" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A197" s="18" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="D197" s="18" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="G197" s="57" t="b">
         <v>1</v>
@@ -11019,14 +11022,14 @@
     </row>
     <row r="198" spans="1:13" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A198" s="60" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B198" s="60" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C198" s="60"/>
       <c r="D198" s="60" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="E198" s="60"/>
       <c r="F198" s="60" t="s">
@@ -11048,13 +11051,13 @@
     </row>
     <row r="199" spans="1:13" s="5" customFormat="1" ht="2.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A199" s="5" t="s">
+        <v>422</v>
+      </c>
+      <c r="B199" s="5" t="s">
+        <v>422</v>
+      </c>
+      <c r="D199" s="5" t="s">
         <v>423</v>
-      </c>
-      <c r="B199" s="5" t="s">
-        <v>423</v>
-      </c>
-      <c r="D199" s="5" t="s">
-        <v>424</v>
       </c>
       <c r="F199" s="61" t="s">
         <v>41</v>
@@ -11071,16 +11074,16 @@
     </row>
     <row r="200" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A200" s="29" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B200" s="29" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="D200" s="29" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="F200" s="29" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="G200" s="64" t="b">
         <v>1</v>
@@ -11094,16 +11097,16 @@
     </row>
     <row r="201" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A201" s="29" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B201" s="29" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="D201" s="29" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="F201" s="29" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="G201" s="64" t="b">
         <v>1</v>
@@ -11117,16 +11120,16 @@
     </row>
     <row r="202" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A202" s="29" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B202" s="29" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D202" s="29" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="F202" s="29" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="G202" s="64" t="b">
         <v>1</v>
@@ -11140,16 +11143,16 @@
     </row>
     <row r="203" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A203" s="29" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B203" s="29" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="D203" s="29" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="F203" s="29" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="G203" s="64" t="b">
         <v>1</v>
@@ -11163,16 +11166,16 @@
     </row>
     <row r="204" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A204" s="29" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B204" s="29" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="D204" s="29" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="F204" s="29" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="G204" s="64" t="b">
         <v>1</v>
@@ -11186,16 +11189,16 @@
     </row>
     <row r="205" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A205" s="29" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B205" s="29" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="D205" s="29" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="F205" s="29" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="G205" s="64" t="b">
         <v>1</v>
@@ -11209,16 +11212,16 @@
     </row>
     <row r="206" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A206" s="29" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B206" s="29" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="D206" s="29" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="F206" s="29" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="G206" s="64" t="b">
         <v>1</v>
@@ -11232,16 +11235,16 @@
     </row>
     <row r="207" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A207" s="29" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B207" s="29" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="D207" s="29" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="F207" s="29" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="G207" s="64" t="b">
         <v>1</v>
@@ -11255,16 +11258,16 @@
     </row>
     <row r="208" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A208" s="29" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B208" s="29" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="D208" s="29" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="F208" s="29" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="G208" s="64" t="b">
         <v>1</v>
@@ -11278,16 +11281,16 @@
     </row>
     <row r="209" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A209" s="29" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B209" s="29" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="D209" s="29" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="F209" s="29" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="G209" s="64" t="b">
         <v>1</v>
@@ -11301,16 +11304,16 @@
     </row>
     <row r="210" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A210" s="29" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B210" s="29" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D210" s="29" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="F210" s="29" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="G210" s="64" t="b">
         <v>1</v>
@@ -11324,16 +11327,16 @@
     </row>
     <row r="211" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A211" s="29" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B211" s="29" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D211" s="29" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="F211" s="29" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="G211" s="64" t="b">
         <v>1</v>
@@ -11347,16 +11350,16 @@
     </row>
     <row r="212" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A212" s="29" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B212" s="29" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="D212" s="29" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="F212" s="29" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="G212" s="64" t="b">
         <v>1</v>
@@ -11370,16 +11373,16 @@
     </row>
     <row r="213" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A213" s="29" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B213" s="29" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="D213" s="29" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="F213" s="29" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="G213" s="64" t="b">
         <v>1</v>
@@ -11393,16 +11396,16 @@
     </row>
     <row r="214" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A214" s="29" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B214" s="29" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D214" s="29" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="F214" s="29" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="G214" s="64" t="b">
         <v>1</v>
@@ -11416,16 +11419,16 @@
     </row>
     <row r="215" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A215" s="29" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B215" s="29" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="D215" s="29" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="F215" s="29" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="G215" s="64" t="b">
         <v>1</v>
@@ -11439,16 +11442,16 @@
     </row>
     <row r="216" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A216" s="29" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B216" s="29" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D216" s="29" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="F216" s="29" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="G216" s="64" t="b">
         <v>1</v>
@@ -11462,16 +11465,16 @@
     </row>
     <row r="217" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A217" s="29" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B217" s="29" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D217" s="29" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="F217" s="29" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="G217" s="64" t="b">
         <v>1</v>
@@ -11485,16 +11488,16 @@
     </row>
     <row r="218" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A218" s="29" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B218" s="29" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D218" s="29" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="F218" s="29" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="G218" s="64" t="b">
         <v>1</v>
@@ -11508,16 +11511,16 @@
     </row>
     <row r="219" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A219" s="29" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B219" s="29" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="D219" s="29" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="F219" s="29" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="G219" s="64" t="b">
         <v>1</v>
@@ -11531,16 +11534,16 @@
     </row>
     <row r="220" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A220" s="29" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B220" s="29" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="D220" s="29" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="F220" s="29" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="G220" s="64" t="b">
         <v>1</v>
@@ -11554,16 +11557,16 @@
     </row>
     <row r="221" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A221" s="29" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B221" s="29" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="D221" s="29" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="F221" s="29" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="G221" s="64" t="b">
         <v>1</v>
@@ -11577,16 +11580,16 @@
     </row>
     <row r="222" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A222" s="29" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B222" s="29" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="D222" s="29" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="F222" s="29" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="G222" s="64" t="b">
         <v>1</v>
@@ -11600,16 +11603,16 @@
     </row>
     <row r="223" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A223" s="29" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B223" s="29" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="D223" s="29" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="F223" s="29" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="G223" s="64" t="b">
         <v>1</v>
@@ -11623,16 +11626,16 @@
     </row>
     <row r="224" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A224" s="29" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B224" s="29" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="D224" s="29" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="F224" s="29" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="G224" s="64" t="b">
         <v>1</v>
@@ -11646,16 +11649,16 @@
     </row>
     <row r="225" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A225" s="29" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B225" s="29" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="D225" s="29" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="F225" s="29" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="G225" s="64" t="b">
         <v>1</v>
@@ -11669,16 +11672,16 @@
     </row>
     <row r="226" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A226" s="29" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B226" s="29" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="D226" s="29" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="F226" s="29" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="G226" s="64" t="b">
         <v>1</v>
@@ -11692,16 +11695,16 @@
     </row>
     <row r="227" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A227" s="29" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B227" s="29" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="D227" s="29" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="F227" s="29" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="G227" s="64" t="b">
         <v>1</v>
@@ -11715,16 +11718,16 @@
     </row>
     <row r="228" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A228" s="29" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B228" s="29" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="D228" s="29" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="F228" s="29" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="G228" s="64" t="b">
         <v>1</v>
@@ -11738,16 +11741,16 @@
     </row>
     <row r="229" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A229" s="29" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B229" s="29" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="D229" s="29" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="F229" s="29" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="G229" s="64" t="b">
         <v>1</v>
@@ -11761,16 +11764,16 @@
     </row>
     <row r="230" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A230" s="29" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B230" s="29" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="D230" s="29" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="F230" s="29" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="G230" s="64" t="b">
         <v>1</v>
@@ -11784,16 +11787,16 @@
     </row>
     <row r="231" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A231" s="29" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B231" s="29" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="D231" s="29" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="F231" s="29" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="G231" s="64" t="b">
         <v>1</v>
@@ -11807,16 +11810,16 @@
     </row>
     <row r="232" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A232" s="29" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B232" s="29" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="D232" s="29" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="F232" s="29" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="G232" s="64" t="b">
         <v>1</v>
@@ -11830,16 +11833,16 @@
     </row>
     <row r="233" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A233" s="29" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B233" s="29" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="D233" s="29" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="F233" s="29" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="G233" s="64" t="b">
         <v>1</v>
@@ -11853,16 +11856,16 @@
     </row>
     <row r="234" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A234" s="29" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B234" s="29" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="D234" s="29" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="F234" s="29" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="G234" s="64" t="b">
         <v>1</v>
@@ -11876,16 +11879,16 @@
     </row>
     <row r="235" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A235" s="29" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B235" s="29" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="D235" s="29" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="F235" s="29" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="G235" s="64" t="b">
         <v>1</v>
@@ -11899,16 +11902,16 @@
     </row>
     <row r="236" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A236" s="29" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B236" s="29" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="D236" s="29" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="F236" s="29" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="G236" s="64" t="b">
         <v>1</v>
@@ -11922,16 +11925,16 @@
     </row>
     <row r="237" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A237" s="29" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B237" s="29" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="D237" s="29" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="F237" s="29" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="G237" s="64" t="b">
         <v>1</v>
@@ -11945,16 +11948,16 @@
     </row>
     <row r="238" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A238" s="29" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B238" s="29" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="D238" s="29" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="F238" s="29" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="G238" s="64" t="b">
         <v>1</v>
@@ -11968,16 +11971,16 @@
     </row>
     <row r="239" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A239" s="29" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B239" s="29" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="D239" s="29" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="F239" s="29" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="G239" s="64" t="b">
         <v>1</v>
@@ -11991,16 +11994,16 @@
     </row>
     <row r="240" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A240" s="29" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B240" s="29" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="D240" s="29" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="F240" s="29" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="G240" s="64" t="b">
         <v>1</v>
@@ -12014,16 +12017,16 @@
     </row>
     <row r="241" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A241" s="29" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B241" s="29" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="D241" s="29" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="F241" s="29" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="G241" s="64" t="b">
         <v>1</v>
@@ -12037,16 +12040,16 @@
     </row>
     <row r="242" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A242" s="29" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B242" s="29" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="D242" s="29" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="F242" s="29" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="G242" s="64" t="b">
         <v>1</v>
@@ -12060,16 +12063,16 @@
     </row>
     <row r="243" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A243" s="29" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B243" s="29" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="D243" s="29" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="F243" s="29" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="G243" s="64" t="b">
         <v>1</v>
@@ -12083,16 +12086,16 @@
     </row>
     <row r="244" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A244" s="29" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B244" s="29" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="D244" s="29" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="F244" s="29" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="G244" s="64" t="b">
         <v>1</v>
@@ -12106,16 +12109,16 @@
     </row>
     <row r="245" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A245" s="29" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B245" s="29" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="D245" s="29" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="F245" s="29" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="G245" s="64" t="b">
         <v>1</v>
@@ -12129,16 +12132,16 @@
     </row>
     <row r="246" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A246" s="29" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B246" s="29" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="D246" s="29" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="F246" s="29" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="G246" s="64" t="b">
         <v>1</v>
@@ -12152,16 +12155,16 @@
     </row>
     <row r="247" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A247" s="29" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="B247" s="29" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="D247" s="29" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="F247" s="29" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="G247" s="64" t="b">
         <v>1</v>
@@ -12175,16 +12178,16 @@
     </row>
     <row r="248" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A248" s="29" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B248" s="29" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="D248" s="29" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="F248" s="29" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="G248" s="64" t="b">
         <v>1</v>
@@ -12198,16 +12201,16 @@
     </row>
     <row r="249" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A249" s="29" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B249" s="29" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="D249" s="29" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="F249" s="29" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="G249" s="64" t="b">
         <v>1</v>
@@ -12221,16 +12224,16 @@
     </row>
     <row r="250" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A250" s="29" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B250" s="29" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="D250" s="29" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="F250" s="29" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="G250" s="64" t="b">
         <v>1</v>
@@ -12244,16 +12247,16 @@
     </row>
     <row r="251" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A251" s="29" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B251" s="29" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="D251" s="29" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="F251" s="29" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="G251" s="64" t="b">
         <v>1</v>
@@ -12267,16 +12270,16 @@
     </row>
     <row r="252" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A252" s="29" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B252" s="29" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="D252" s="29" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="F252" s="29" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="G252" s="64" t="b">
         <v>1</v>
@@ -12290,16 +12293,16 @@
     </row>
     <row r="253" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A253" s="29" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B253" s="29" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="D253" s="29" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="F253" s="29" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="G253" s="64" t="b">
         <v>1</v>
@@ -12313,16 +12316,16 @@
     </row>
     <row r="254" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A254" s="29" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B254" s="29" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="D254" s="29" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="F254" s="29" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="G254" s="64" t="b">
         <v>1</v>
@@ -12336,16 +12339,16 @@
     </row>
     <row r="255" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A255" s="29" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="B255" s="29" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="D255" s="29" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="F255" s="29" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="G255" s="64" t="b">
         <v>1</v>
@@ -12359,16 +12362,16 @@
     </row>
     <row r="256" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A256" s="29" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B256" s="29" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D256" s="29" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="F256" s="29" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="G256" s="64" t="b">
         <v>1</v>
@@ -12382,16 +12385,16 @@
     </row>
     <row r="257" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A257" s="29" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B257" s="29" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="D257" s="29" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="F257" s="29" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="G257" s="64" t="b">
         <v>1</v>
@@ -12405,16 +12408,16 @@
     </row>
     <row r="258" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A258" s="29" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B258" s="29" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="D258" s="29" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F258" s="29" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="G258" s="64" t="b">
         <v>1</v>
@@ -12428,16 +12431,16 @@
     </row>
     <row r="259" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A259" s="29" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B259" s="29" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="D259" s="29" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="F259" s="29" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="G259" s="64" t="b">
         <v>1</v>
@@ -12451,16 +12454,16 @@
     </row>
     <row r="260" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A260" s="29" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B260" s="29" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="D260" s="29" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="F260" s="29" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="G260" s="64" t="b">
         <v>1</v>
@@ -12474,16 +12477,16 @@
     </row>
     <row r="261" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A261" s="29" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B261" s="29" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D261" s="29" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="F261" s="29" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="G261" s="64" t="b">
         <v>1</v>
@@ -12497,16 +12500,16 @@
     </row>
     <row r="262" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A262" s="29" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="B262" s="29" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D262" s="29" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="F262" s="29" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="G262" s="64" t="b">
         <v>1</v>
@@ -12520,16 +12523,16 @@
     </row>
     <row r="263" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A263" s="29" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="B263" s="29" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="D263" s="29" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="F263" s="29" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="G263" s="64" t="b">
         <v>1</v>
@@ -12543,16 +12546,16 @@
     </row>
     <row r="264" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A264" s="29" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B264" s="29" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="D264" s="29" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="F264" s="29" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="G264" s="64" t="b">
         <v>1</v>
@@ -12566,16 +12569,16 @@
     </row>
     <row r="265" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A265" s="29" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="B265" s="29" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D265" s="29" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="F265" s="29" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="G265" s="64" t="b">
         <v>1</v>
@@ -12589,16 +12592,16 @@
     </row>
     <row r="266" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A266" s="29" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="B266" s="29" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="D266" s="29" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="F266" s="29" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="G266" s="64" t="b">
         <v>1</v>
@@ -12612,16 +12615,16 @@
     </row>
     <row r="267" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A267" s="29" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="B267" s="29" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="D267" s="29" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="F267" s="29" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="G267" s="64" t="b">
         <v>1</v>
@@ -12635,13 +12638,13 @@
     </row>
     <row r="268" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A268" s="29" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="B268" s="29" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="D268" s="29" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="G268" s="64" t="b">
         <v>1</v>
@@ -12655,16 +12658,16 @@
     </row>
     <row r="269" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A269" s="29" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B269" s="29" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="D269" s="29" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F269" s="29" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G269" s="64" t="b">
         <v>1</v>
@@ -12678,16 +12681,16 @@
     </row>
     <row r="270" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A270" s="29" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="B270" s="29" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="D270" s="29" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="F270" s="29" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G270" s="64" t="b">
         <v>1</v>
@@ -12701,16 +12704,16 @@
     </row>
     <row r="271" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A271" s="29" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B271" s="29" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="D271" s="29" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="F271" s="29" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G271" s="64" t="b">
         <v>1</v>
@@ -12724,16 +12727,16 @@
     </row>
     <row r="272" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A272" s="29" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B272" s="29" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="D272" s="29" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="F272" s="29" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G272" s="64" t="b">
         <v>1</v>
@@ -12747,16 +12750,16 @@
     </row>
     <row r="273" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A273" s="29" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="B273" s="29" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D273" s="29" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F273" s="29" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G273" s="64" t="b">
         <v>1</v>
@@ -12770,16 +12773,16 @@
     </row>
     <row r="274" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A274" s="29" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B274" s="29" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="D274" s="29" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="F274" s="29" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G274" s="64" t="b">
         <v>1</v>
@@ -12793,16 +12796,16 @@
     </row>
     <row r="275" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A275" s="29" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="B275" s="29" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="D275" s="29" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="F275" s="29" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="G275" s="64" t="b">
         <v>1</v>
@@ -12816,16 +12819,16 @@
     </row>
     <row r="276" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A276" s="29" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="B276" s="29" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="D276" s="29" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="F276" s="29" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="G276" s="64" t="b">
         <v>1</v>
@@ -12839,16 +12842,16 @@
     </row>
     <row r="277" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A277" s="29" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B277" s="29" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="D277" s="29" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="F277" s="29" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="G277" s="64" t="b">
         <v>1</v>
@@ -12862,16 +12865,16 @@
     </row>
     <row r="278" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A278" s="29" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B278" s="29" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="D278" s="29" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="F278" s="29" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="G278" s="64" t="b">
         <v>1</v>
@@ -12885,16 +12888,16 @@
     </row>
     <row r="279" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A279" s="29" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B279" s="29" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="D279" s="29" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="F279" s="29" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G279" s="64" t="b">
         <v>1</v>
@@ -12908,16 +12911,16 @@
     </row>
     <row r="280" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A280" s="29" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="B280" s="29" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="D280" s="29" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="F280" s="29" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G280" s="64" t="b">
         <v>1</v>
@@ -12931,16 +12934,16 @@
     </row>
     <row r="281" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A281" s="29" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="B281" s="29" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="D281" s="29" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="F281" s="29" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="G281" s="64" t="b">
         <v>1</v>
@@ -12954,16 +12957,16 @@
     </row>
     <row r="282" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A282" s="29" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="B282" s="29" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="D282" s="29" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="F282" s="29" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="G282" s="64" t="b">
         <v>1</v>
@@ -12977,16 +12980,16 @@
     </row>
     <row r="283" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A283" s="29" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="B283" s="29" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="D283" s="29" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="F283" s="29" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="G283" s="64" t="b">
         <v>1</v>
@@ -13000,16 +13003,16 @@
     </row>
     <row r="284" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A284" s="29" t="s">
+        <v>553</v>
+      </c>
+      <c r="B284" s="29" t="s">
+        <v>553</v>
+      </c>
+      <c r="D284" s="29" t="s">
+        <v>553</v>
+      </c>
+      <c r="F284" s="29" t="s">
         <v>554</v>
-      </c>
-      <c r="B284" s="29" t="s">
-        <v>554</v>
-      </c>
-      <c r="D284" s="29" t="s">
-        <v>554</v>
-      </c>
-      <c r="F284" s="29" t="s">
-        <v>555</v>
       </c>
       <c r="G284" s="64" t="b">
         <v>1</v>
@@ -13023,16 +13026,16 @@
     </row>
     <row r="285" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A285" s="29" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="B285" s="29" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="D285" s="29" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="F285" s="29" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="G285" s="64" t="b">
         <v>1</v>
@@ -13561,7 +13564,7 @@
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J28" sqref="J28:K28"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13571,15 +13574,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="67" t="s">
+        <v>521</v>
+      </c>
+      <c r="B1" t="s">
         <v>522</v>
-      </c>
-      <c r="B1" t="s">
-        <v>523</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="67" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="B2" t="s">
         <v>230</v>
@@ -13590,106 +13593,106 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="67" t="s">
+        <v>524</v>
+      </c>
+      <c r="B4" t="s">
         <v>525</v>
-      </c>
-      <c r="B4" t="s">
-        <v>526</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="67" t="s">
+        <v>526</v>
+      </c>
+      <c r="B5" t="s">
         <v>527</v>
-      </c>
-      <c r="B5" t="s">
-        <v>528</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="67" t="s">
+        <v>528</v>
+      </c>
+      <c r="B6" t="s">
         <v>529</v>
-      </c>
-      <c r="B6" t="s">
-        <v>530</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="67" t="s">
+        <v>530</v>
+      </c>
+      <c r="B7" t="s">
         <v>531</v>
-      </c>
-      <c r="B7" t="s">
-        <v>532</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="67" t="s">
+        <v>532</v>
+      </c>
+      <c r="B8" t="s">
         <v>533</v>
-      </c>
-      <c r="B8" t="s">
-        <v>534</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="67" t="s">
+        <v>534</v>
+      </c>
+      <c r="B9" t="s">
         <v>535</v>
-      </c>
-      <c r="B9" t="s">
-        <v>536</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="67" t="s">
+        <v>536</v>
+      </c>
+      <c r="B10" t="s">
         <v>537</v>
-      </c>
-      <c r="B10" t="s">
-        <v>538</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="67" t="s">
+        <v>538</v>
+      </c>
+      <c r="B11" t="s">
         <v>539</v>
-      </c>
-      <c r="B11" t="s">
-        <v>540</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="67" t="s">
+        <v>540</v>
+      </c>
+      <c r="B12" t="s">
         <v>541</v>
-      </c>
-      <c r="B12" t="s">
-        <v>542</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="67" t="s">
+        <v>542</v>
+      </c>
+      <c r="B13" t="s">
         <v>543</v>
-      </c>
-      <c r="B13" t="s">
-        <v>544</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="67" t="s">
+        <v>544</v>
+      </c>
+      <c r="B14" t="s">
         <v>545</v>
-      </c>
-      <c r="B14" t="s">
-        <v>546</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="67" t="s">
+        <v>546</v>
+      </c>
+      <c r="B15" t="s">
         <v>547</v>
-      </c>
-      <c r="B15" t="s">
-        <v>548</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="67" t="s">
+        <v>548</v>
+      </c>
+      <c r="B16" t="s">
         <v>549</v>
-      </c>
-      <c r="B16" t="s">
-        <v>550</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -13700,10 +13703,10 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="67" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="B19" t="s">
-        <v>231</v>
+        <v>556</v>
       </c>
     </row>
   </sheetData>

</xml_diff>